<commit_message>
Framework is almost done, only clearation work is left
</commit_message>
<xml_diff>
--- a/src/test/resources/excels/testdata.xlsx
+++ b/src/test/resources/excels/testdata.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="25380" windowHeight="11640"/>
+    <workbookView windowWidth="25380" windowHeight="11640" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="RUNMANAGER" sheetId="1" r:id="rId1"/>
+    <sheet name="DATA" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="34">
   <si>
     <t>testname</t>
   </si>
@@ -50,6 +51,72 @@
   </si>
   <si>
     <t>2</t>
+  </si>
+  <si>
+    <t>googleSearchTest</t>
+  </si>
+  <si>
+    <t>To check whether Google search is working</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>enterAdminPageTest</t>
+  </si>
+  <si>
+    <t>To check whether use can enter Admin page</t>
+  </si>
+  <si>
+    <t>enterPIMPageTest</t>
+  </si>
+  <si>
+    <t>To check whether use can enter PIM page</t>
+  </si>
+  <si>
+    <t>browser</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>fname</t>
+  </si>
+  <si>
+    <t>searchText</t>
+  </si>
+  <si>
+    <t>chrome</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>admin123</t>
+  </si>
+  <si>
+    <t>Oscar</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>edge</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Admin123</t>
+  </si>
+  <si>
+    <t>Automation</t>
+  </si>
+  <si>
+    <t>QA</t>
   </si>
 </sst>
 </file>
@@ -670,6 +737,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1197,15 +1267,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="2" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="5" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="13.9296875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.75" style="1" customWidth="1"/>
     <col min="2" max="2" width="51.953125" style="1" customWidth="1"/>
     <col min="3" max="16384" width="9" style="1"/>
   </cols>
@@ -1261,6 +1331,307 @@
         <v>8</v>
       </c>
     </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="6"/>
+  <cols>
+    <col min="1" max="1" width="18.6171875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" customFormat="1" spans="1:7">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Finish building the Framework
</commit_message>
<xml_diff>
--- a/src/test/resources/excels/testdata.xlsx
+++ b/src/test/resources/excels/testdata.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="35">
   <si>
     <t>testname</t>
   </si>
@@ -44,79 +44,82 @@
     <t>1</t>
   </si>
   <si>
+    <t>enterAdminPageTest</t>
+  </si>
+  <si>
+    <t>To check whether use can enter Admin page</t>
+  </si>
+  <si>
+    <t>enterPIMPageTest</t>
+  </si>
+  <si>
+    <t>To check whether use can enter PIM page</t>
+  </si>
+  <si>
+    <t>baiduSearchTest</t>
+  </si>
+  <si>
+    <t>To check whether baidu search is working</t>
+  </si>
+  <si>
+    <t>browser</t>
+  </si>
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>fname</t>
+  </si>
+  <si>
+    <t>searchText</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>chrome</t>
+  </si>
+  <si>
+    <t>116.0</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>YWRtaW4xMjM=</t>
+  </si>
+  <si>
+    <t>Oscar</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>firefox</t>
+  </si>
+  <si>
     <t>newTest</t>
   </si>
   <si>
-    <t>To check whether this test is executed</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>googleSearchTest</t>
-  </si>
-  <si>
-    <t>To check whether Google search is working</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>enterAdminPageTest</t>
-  </si>
-  <si>
-    <t>To check whether use can enter Admin page</t>
-  </si>
-  <si>
-    <t>enterPIMPageTest</t>
-  </si>
-  <si>
-    <t>To check whether use can enter PIM page</t>
-  </si>
-  <si>
-    <t>browser</t>
-  </si>
-  <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>fname</t>
-  </si>
-  <si>
-    <t>searchText</t>
-  </si>
-  <si>
-    <t>chrome</t>
-  </si>
-  <si>
-    <t>Admin</t>
-  </si>
-  <si>
-    <t>admin123</t>
-  </si>
-  <si>
-    <t>Oscar</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
     <t>edge</t>
   </si>
   <si>
-    <t>no</t>
-  </si>
-  <si>
     <t>Admin123</t>
   </si>
   <si>
+    <t>115.0</t>
+  </si>
+  <si>
     <t>Automation</t>
   </si>
   <si>
-    <t>QA</t>
+    <t>Hello world</t>
   </si>
 </sst>
 </file>
@@ -1267,13 +1270,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="5" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="4" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="15.75" style="1" customWidth="1"/>
     <col min="2" max="2" width="51.953125" style="1" customWidth="1"/>
@@ -1325,24 +1328,24 @@
         <v>7</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>8</v>
@@ -1350,10 +1353,10 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>7</v>
@@ -1362,23 +1365,6 @@
         <v>8</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1391,18 +1377,19 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="18.6171875" customWidth="1"/>
+    <col min="6" max="6" width="17.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1410,226 +1397,256 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
         <v>20</v>
       </c>
-      <c r="E1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" t="s">
-        <v>23</v>
-      </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
         <v>24</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>25</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>26</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>28</v>
-      </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
         <v>29</v>
       </c>
-      <c r="D3" t="s">
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" t="s">
         <v>25</v>
       </c>
-      <c r="E3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="G4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>28</v>
+      <c r="H4" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" t="s">
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
         <v>29</v>
       </c>
-      <c r="D4" t="s">
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" t="s">
         <v>25</v>
       </c>
-      <c r="E4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>28</v>
+      <c r="G5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" customFormat="1" spans="1:7">
+    <row r="6" customFormat="1" spans="1:8">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
         <v>7</v>
       </c>
-      <c r="C6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" t="s">
         <v>26</v>
       </c>
-      <c r="F6" t="s">
+      <c r="H7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="F8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="D10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="G7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" t="s">
-        <v>27</v>
-      </c>
-      <c r="G8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" t="s">
-        <v>26</v>
-      </c>
-      <c r="F9" t="s">
-        <v>27</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" t="s">
-        <v>26</v>
-      </c>
-      <c r="F10" t="s">
-        <v>27</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>